<commit_message>
changes for parallel execution
</commit_message>
<xml_diff>
--- a/src/test/resources/BooksAPIs_TestData.xlsx
+++ b/src/test/resources/BooksAPIs_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Numpy Ninja\BooksAPI_RestAssured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0B9A52-A79A-4473-BF88-AA8E6063E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167FE159-E432-41D6-905B-DC9F00255437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="3324" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
   <si>
     <t>scenario</t>
   </si>
@@ -121,13 +121,37 @@
   </si>
   <si>
     <t>James Donnas</t>
+  </si>
+  <si>
+    <t>post order background</t>
+  </si>
+  <si>
+    <t>test name1</t>
+  </si>
+  <si>
+    <t>test name2</t>
+  </si>
+  <si>
+    <t>test name3</t>
+  </si>
+  <si>
+    <t>test name4</t>
+  </si>
+  <si>
+    <t>test name5</t>
+  </si>
+  <si>
+    <t>test name6</t>
+  </si>
+  <si>
+    <t>test name7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +164,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -446,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,14 +511,14 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>31</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
@@ -498,14 +528,14 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>31</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>14</v>
@@ -515,11 +545,14 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>14</v>
@@ -529,11 +562,14 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
@@ -543,20 +579,134 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -730,7 +880,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>